<commit_message>
Cleaned up repository, excluded version control of .su and .o files, excluded TouchGFX/simulator & /generated files. Commited recent code with UI with relay settings.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="81">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -141,6 +141,123 @@
   </si>
   <si>
     <t xml:space="preserve">Small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Relay &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rele &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&gt; ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zamik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dolzina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;digit&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">romand__.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relay 1 Setup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OratorStd.otf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relay 2 Setup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relay 3 Setup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isocpeur.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rele 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rele 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rele 3</t>
   </si>
 </sst>
 </file>
@@ -1371,7 +1488,7 @@
         <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="D4">
         <v>20</v>
@@ -1384,7 +1501,9 @@
       </c>
       <c r="G4"/>
       <c r="H4"/>
-      <c r="I4"/>
+      <c r="I4" t="s">
+        <v>42</v>
+      </c>
       <c r="J4"/>
       <c r="L4" s="4" t="s">
         <v>9</v>
@@ -1407,10 +1526,10 @@
         <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="D5">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -1420,7 +1539,9 @@
       </c>
       <c r="G5"/>
       <c r="H5"/>
-      <c r="I5"/>
+      <c r="I5" t="s">
+        <v>42</v>
+      </c>
       <c r="J5"/>
       <c r="L5" s="7" t="s">
         <v>1</v>
@@ -1600,6 +1721,269 @@
       <c r="F3" t="s">
         <v>36</v>
       </c>
+      <c r="G3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" t="s">
+        <v>76</v>
+      </c>
+      <c r="G16" t="s">
+        <v>80</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Version with a working long press button
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="103">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -258,6 +258,72 @@
   </si>
   <si>
     <t xml:space="preserve">Rele 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId36</t>
   </si>
 </sst>
 </file>
@@ -1985,6 +2051,246 @@
         <v>80</v>
       </c>
     </row>
+    <row r="17">
+      <c r="B17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" t="s">
+        <v>85</v>
+      </c>
+      <c r="G19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" t="s">
+        <v>85</v>
+      </c>
+      <c r="G20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" t="s">
+        <v>72</v>
+      </c>
+      <c r="G22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" t="s">
+        <v>85</v>
+      </c>
+      <c r="G23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" t="s">
+        <v>85</v>
+      </c>
+      <c r="G24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" t="s">
+        <v>59</v>
+      </c>
+      <c r="G25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" t="s">
+        <v>72</v>
+      </c>
+      <c r="G26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" t="s">
+        <v>85</v>
+      </c>
+      <c r="G27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" t="s">
+        <v>51</v>
+      </c>
+      <c r="E28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" t="s">
+        <v>85</v>
+      </c>
+      <c r="G28" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Added first task function and implemented queue. Added lots of GUI elements, all working as expected for now.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1986" uniqueCount="119">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -324,6 +324,54 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xlarge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trajanje</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt; pcs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt; mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Length setup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mm</t>
   </si>
 </sst>
 </file>
@@ -1658,6 +1706,27 @@
       <c r="P6" s="10"/>
     </row>
     <row r="7" spans="2:16">
+      <c r="B7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7">
+        <v>40</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7"/>
       <c r="L7" s="7" t="s">
         <v>7</v>
       </c>
@@ -1948,7 +2017,7 @@
         <v>72</v>
       </c>
       <c r="G11" t="s">
-        <v>64</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12">
@@ -2056,7 +2125,7 @@
         <v>81</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D17" t="s">
         <v>82</v>
@@ -2068,7 +2137,7 @@
         <v>59</v>
       </c>
       <c r="G17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18">
@@ -2076,7 +2145,7 @@
         <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
         <v>82</v>
@@ -2088,7 +2157,7 @@
         <v>72</v>
       </c>
       <c r="G18" t="s">
-        <v>63</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19">
@@ -2096,7 +2165,7 @@
         <v>84</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
         <v>51</v>
@@ -2108,7 +2177,7 @@
         <v>85</v>
       </c>
       <c r="G19" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20">
@@ -2116,7 +2185,7 @@
         <v>86</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D20" t="s">
         <v>51</v>
@@ -2128,7 +2197,7 @@
         <v>85</v>
       </c>
       <c r="G20" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21">
@@ -2136,7 +2205,7 @@
         <v>95</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D21" t="s">
         <v>82</v>
@@ -2148,7 +2217,7 @@
         <v>59</v>
       </c>
       <c r="G21" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22">
@@ -2156,7 +2225,7 @@
         <v>96</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D22" t="s">
         <v>82</v>
@@ -2168,7 +2237,7 @@
         <v>72</v>
       </c>
       <c r="G22" t="s">
-        <v>63</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23">
@@ -2176,7 +2245,7 @@
         <v>97</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D23" t="s">
         <v>51</v>
@@ -2188,7 +2257,7 @@
         <v>85</v>
       </c>
       <c r="G23" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24">
@@ -2196,7 +2265,7 @@
         <v>98</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D24" t="s">
         <v>51</v>
@@ -2208,7 +2277,7 @@
         <v>85</v>
       </c>
       <c r="G24" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25">
@@ -2216,7 +2285,7 @@
         <v>99</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D25" t="s">
         <v>82</v>
@@ -2228,7 +2297,7 @@
         <v>59</v>
       </c>
       <c r="G25" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26">
@@ -2236,7 +2305,7 @@
         <v>100</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D26" t="s">
         <v>82</v>
@@ -2248,7 +2317,7 @@
         <v>72</v>
       </c>
       <c r="G26" t="s">
-        <v>63</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27">
@@ -2256,7 +2325,7 @@
         <v>101</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D27" t="s">
         <v>51</v>
@@ -2268,7 +2337,7 @@
         <v>85</v>
       </c>
       <c r="G27" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28">
@@ -2276,7 +2345,7 @@
         <v>102</v>
       </c>
       <c r="C28" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D28" t="s">
         <v>51</v>
@@ -2288,7 +2357,167 @@
         <v>85</v>
       </c>
       <c r="G28" t="s">
-        <v>63</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" t="s">
+        <v>103</v>
+      </c>
+      <c r="D29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" t="s">
+        <v>46</v>
+      </c>
+      <c r="F29" t="s">
+        <v>109</v>
+      </c>
+      <c r="G29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" t="s">
+        <v>46</v>
+      </c>
+      <c r="F30" t="s">
+        <v>52</v>
+      </c>
+      <c r="G30" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="s">
+        <v>110</v>
+      </c>
+      <c r="C31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" t="s">
+        <v>45</v>
+      </c>
+      <c r="E31" t="s">
+        <v>46</v>
+      </c>
+      <c r="F31" t="s">
+        <v>111</v>
+      </c>
+      <c r="G31" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" t="s">
+        <v>51</v>
+      </c>
+      <c r="E32" t="s">
+        <v>46</v>
+      </c>
+      <c r="F32" t="s">
+        <v>52</v>
+      </c>
+      <c r="G32" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" t="s">
+        <v>45</v>
+      </c>
+      <c r="E33" t="s">
+        <v>46</v>
+      </c>
+      <c r="F33" t="s">
+        <v>111</v>
+      </c>
+      <c r="G33" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" t="s">
+        <v>51</v>
+      </c>
+      <c r="E34" t="s">
+        <v>46</v>
+      </c>
+      <c r="F34" t="s">
+        <v>52</v>
+      </c>
+      <c r="G34" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="s">
+        <v>115</v>
+      </c>
+      <c r="C35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" t="s">
+        <v>51</v>
+      </c>
+      <c r="E35" t="s">
+        <v>46</v>
+      </c>
+      <c r="F35" t="s">
+        <v>116</v>
+      </c>
+      <c r="G35" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="s">
+        <v>117</v>
+      </c>
+      <c r="C36" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" t="s">
+        <v>51</v>
+      </c>
+      <c r="E36" t="s">
+        <v>46</v>
+      </c>
+      <c r="F36" t="s">
+        <v>118</v>
+      </c>
+      <c r="G36" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added some GUI elements. Pop up status information messaging system.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1986" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4882" uniqueCount="160">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -372,6 +372,129 @@
   </si>
   <si>
     <t xml:space="preserve">mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StatusMsgDelayOF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum of delay and duration cannot exceed 42 seconds. The delay was trimmed and relay will never be turned on.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vsota zamika in trajanja ne sme preseči 42 sekund. Zamik je bil obrezan in rele ne bo nikoli vklopljen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StatusMsgDurationOF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum of delay and duration cannot exceed 42 seconds. The duration was trimmed and relay will be turned off earlier.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vsota zamika in trajanja ne sme preseči 42 sekund. Trajanje je bilo omejeno in rele bo izklopljen predčasno.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StatusMsgRelayDeactivated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duration is 0. Relay is now inactive.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trajanje je 0. Rele je neaktiven.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATUSMSG_DELAY_OF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATUSMSG_DURATION_OF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATUSMSG_RELAY_DEACTIVATED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XXLarge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum of delay and duration should not exceed 42 seconds. The delay was trimmed and relay will never be turned on.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum of delay and duration should not exceed 42 seconds. The duration was trimmed and relay will be turned off earlier.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATUSMSG_SET_LENGTH_TRIMMED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum allowed length is 10000 mm. The length was trimmmed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Najdaljsa dovoljena dolzina je 10000 mm. Dolzina je bila skrajsana.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATUSMSG_OTHER_ERR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unhandled error.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neznana napaka.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status id: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SLO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt; m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt; kos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ponastavi</t>
   </si>
 </sst>
 </file>
@@ -1676,7 +1799,7 @@
         <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="D6">
         <v>10</v>
@@ -1744,6 +1867,27 @@
       </c>
     </row>
     <row r="8" spans="2:16">
+      <c r="B8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8">
+        <v>60</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8"/>
       <c r="L8" s="7" t="s">
         <v>8</v>
       </c>
@@ -2377,7 +2521,7 @@
         <v>109</v>
       </c>
       <c r="G29" t="s">
-        <v>105</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30">
@@ -2397,7 +2541,7 @@
         <v>52</v>
       </c>
       <c r="G30" t="s">
-        <v>107</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31">
@@ -2417,7 +2561,7 @@
         <v>111</v>
       </c>
       <c r="G31" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32">
@@ -2437,7 +2581,7 @@
         <v>52</v>
       </c>
       <c r="G32" t="s">
-        <v>107</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33">
@@ -2457,7 +2601,7 @@
         <v>111</v>
       </c>
       <c r="G33" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34">
@@ -2477,7 +2621,7 @@
         <v>52</v>
       </c>
       <c r="G34" t="s">
-        <v>107</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35">
@@ -2518,6 +2662,326 @@
       </c>
       <c r="G36" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="s">
+        <v>129</v>
+      </c>
+      <c r="C37" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" t="s">
+        <v>45</v>
+      </c>
+      <c r="E37" t="s">
+        <v>46</v>
+      </c>
+      <c r="F37" t="s">
+        <v>133</v>
+      </c>
+      <c r="G37" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="s">
+        <v>130</v>
+      </c>
+      <c r="C38" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" t="s">
+        <v>45</v>
+      </c>
+      <c r="E38" t="s">
+        <v>46</v>
+      </c>
+      <c r="F38" t="s">
+        <v>134</v>
+      </c>
+      <c r="G38" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="s">
+        <v>131</v>
+      </c>
+      <c r="C39" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" t="s">
+        <v>45</v>
+      </c>
+      <c r="E39" t="s">
+        <v>46</v>
+      </c>
+      <c r="F39" t="s">
+        <v>127</v>
+      </c>
+      <c r="G39" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="s">
+        <v>135</v>
+      </c>
+      <c r="C40" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40" t="s">
+        <v>45</v>
+      </c>
+      <c r="E40" t="s">
+        <v>46</v>
+      </c>
+      <c r="F40" t="s">
+        <v>136</v>
+      </c>
+      <c r="G40" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" t="s">
+        <v>138</v>
+      </c>
+      <c r="C41" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" t="s">
+        <v>45</v>
+      </c>
+      <c r="E41" t="s">
+        <v>46</v>
+      </c>
+      <c r="F41" t="s">
+        <v>139</v>
+      </c>
+      <c r="G41" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" t="s">
+        <v>41</v>
+      </c>
+      <c r="D42" t="s">
+        <v>45</v>
+      </c>
+      <c r="E42" t="s">
+        <v>46</v>
+      </c>
+      <c r="F42" t="s">
+        <v>141</v>
+      </c>
+      <c r="G42" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="s">
+        <v>142</v>
+      </c>
+      <c r="C43" t="s">
+        <v>41</v>
+      </c>
+      <c r="D43" t="s">
+        <v>51</v>
+      </c>
+      <c r="E43" t="s">
+        <v>46</v>
+      </c>
+      <c r="F43" t="s">
+        <v>52</v>
+      </c>
+      <c r="G43" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="B44" t="s">
+        <v>143</v>
+      </c>
+      <c r="C44" t="s">
+        <v>40</v>
+      </c>
+      <c r="D44" t="s">
+        <v>51</v>
+      </c>
+      <c r="E44" t="s">
+        <v>46</v>
+      </c>
+      <c r="F44" t="s">
+        <v>63</v>
+      </c>
+      <c r="G44" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" t="s">
+        <v>144</v>
+      </c>
+      <c r="C45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D45" t="s">
+        <v>51</v>
+      </c>
+      <c r="E45" t="s">
+        <v>46</v>
+      </c>
+      <c r="F45" t="s">
+        <v>145</v>
+      </c>
+      <c r="G45" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" t="s">
+        <v>146</v>
+      </c>
+      <c r="C46" t="s">
+        <v>40</v>
+      </c>
+      <c r="D46" t="s">
+        <v>45</v>
+      </c>
+      <c r="E46" t="s">
+        <v>46</v>
+      </c>
+      <c r="F46" t="s">
+        <v>147</v>
+      </c>
+      <c r="G46" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" t="s">
+        <v>148</v>
+      </c>
+      <c r="C47" t="s">
+        <v>40</v>
+      </c>
+      <c r="D47" t="s">
+        <v>51</v>
+      </c>
+      <c r="E47" t="s">
+        <v>46</v>
+      </c>
+      <c r="F47" t="s">
+        <v>118</v>
+      </c>
+      <c r="G47" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" t="s">
+        <v>149</v>
+      </c>
+      <c r="C48" t="s">
+        <v>40</v>
+      </c>
+      <c r="D48" t="s">
+        <v>51</v>
+      </c>
+      <c r="E48" t="s">
+        <v>46</v>
+      </c>
+      <c r="F48" t="s">
+        <v>145</v>
+      </c>
+      <c r="G48" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" t="s">
+        <v>150</v>
+      </c>
+      <c r="C49" t="s">
+        <v>40</v>
+      </c>
+      <c r="D49" t="s">
+        <v>45</v>
+      </c>
+      <c r="E49" t="s">
+        <v>46</v>
+      </c>
+      <c r="F49" t="s">
+        <v>151</v>
+      </c>
+      <c r="G49" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="s">
+        <v>152</v>
+      </c>
+      <c r="C50" t="s">
+        <v>132</v>
+      </c>
+      <c r="D50" t="s">
+        <v>45</v>
+      </c>
+      <c r="E50" t="s">
+        <v>46</v>
+      </c>
+      <c r="F50" t="s">
+        <v>155</v>
+      </c>
+      <c r="G50" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" t="s">
+        <v>154</v>
+      </c>
+      <c r="C51" t="s">
+        <v>132</v>
+      </c>
+      <c r="D51" t="s">
+        <v>51</v>
+      </c>
+      <c r="E51" t="s">
+        <v>46</v>
+      </c>
+      <c r="F51" t="s">
+        <v>52</v>
+      </c>
+      <c r="G51" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52" t="s">
+        <v>156</v>
+      </c>
+      <c r="C52" t="s">
+        <v>40</v>
+      </c>
+      <c r="D52" t="s">
+        <v>45</v>
+      </c>
+      <c r="E52" t="s">
+        <v>46</v>
+      </c>
+      <c r="F52" t="s">
+        <v>157</v>
+      </c>
+      <c r="G52" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Save and load from memory. Still problem with set length saving into memory.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4882" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6604" uniqueCount="167">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -495,6 +495,27 @@
   </si>
   <si>
     <t xml:space="preserve">Ponastavi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATUSMSG_SETTINGS_LOAD_ERR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Settings could not be loaded from non-volatile memory. Manually set parameters.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nastavitve niso bile uspesno vnesene. Nastavi rocno,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATUSMSG_SETTINGS_SAVE_ERR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error writing to memory. Try again or reset the device.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pisanje v spomin je bilo neuspesno. Poskusi ponovno ali resetiraj napravo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.",</t>
   </si>
 </sst>
 </file>
@@ -1736,7 +1757,9 @@
       <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="G4"/>
+      <c r="G4" t="s">
+        <v>166</v>
+      </c>
       <c r="H4"/>
       <c r="I4" t="s">
         <v>42</v>
@@ -1774,7 +1797,9 @@
       <c r="F5" t="s">
         <v>17</v>
       </c>
-      <c r="G5"/>
+      <c r="G5" t="s">
+        <v>166</v>
+      </c>
       <c r="H5"/>
       <c r="I5" t="s">
         <v>42</v>
@@ -1810,9 +1835,13 @@
       <c r="F6" t="s">
         <v>17</v>
       </c>
-      <c r="G6"/>
+      <c r="G6" t="s">
+        <v>166</v>
+      </c>
       <c r="H6"/>
-      <c r="I6"/>
+      <c r="I6" t="s">
+        <v>42</v>
+      </c>
       <c r="J6"/>
       <c r="L6" s="7" t="s">
         <v>2</v>
@@ -1844,7 +1873,9 @@
       <c r="F7" t="s">
         <v>17</v>
       </c>
-      <c r="G7"/>
+      <c r="G7" t="s">
+        <v>166</v>
+      </c>
       <c r="H7"/>
       <c r="I7" t="s">
         <v>42</v>
@@ -1882,7 +1913,9 @@
       <c r="F8" t="s">
         <v>17</v>
       </c>
-      <c r="G8"/>
+      <c r="G8" t="s">
+        <v>166</v>
+      </c>
       <c r="H8"/>
       <c r="I8" t="s">
         <v>42</v>
@@ -2984,6 +3017,46 @@
         <v>159</v>
       </c>
     </row>
+    <row r="53">
+      <c r="B53" t="s">
+        <v>160</v>
+      </c>
+      <c r="C53" t="s">
+        <v>38</v>
+      </c>
+      <c r="D53" t="s">
+        <v>45</v>
+      </c>
+      <c r="E53" t="s">
+        <v>46</v>
+      </c>
+      <c r="F53" t="s">
+        <v>161</v>
+      </c>
+      <c r="G53" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="B54" t="s">
+        <v>163</v>
+      </c>
+      <c r="C54" t="s">
+        <v>38</v>
+      </c>
+      <c r="D54" t="s">
+        <v>45</v>
+      </c>
+      <c r="E54" t="s">
+        <v>46</v>
+      </c>
+      <c r="F54" t="s">
+        <v>164</v>
+      </c>
+      <c r="G54" t="s">
+        <v>165</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
EEPROM save data now works (with a delay instead of ACK polling), added error eeprom report on screen.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6604" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8824" uniqueCount="171">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -516,6 +516,18 @@
   </si>
   <si>
     <t xml:space="preserve">.",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,A-Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.",ABCDEFGHIJKLMNOPRQSTUVZWY_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.",_</t>
   </si>
 </sst>
 </file>
@@ -1764,7 +1776,9 @@
       <c r="I4" t="s">
         <v>42</v>
       </c>
-      <c r="J4"/>
+      <c r="J4" t="s">
+        <v>107</v>
+      </c>
       <c r="L4" s="4" t="s">
         <v>9</v>
       </c>
@@ -1804,7 +1818,9 @@
       <c r="I5" t="s">
         <v>42</v>
       </c>
-      <c r="J5"/>
+      <c r="J5" t="s">
+        <v>107</v>
+      </c>
       <c r="L5" s="7" t="s">
         <v>1</v>
       </c>
@@ -1836,13 +1852,15 @@
         <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="H6"/>
       <c r="I6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J6"/>
+        <v>167</v>
+      </c>
+      <c r="J6" t="s">
+        <v>107</v>
+      </c>
       <c r="L6" s="7" t="s">
         <v>2</v>
       </c>
@@ -1880,7 +1898,9 @@
       <c r="I7" t="s">
         <v>42</v>
       </c>
-      <c r="J7"/>
+      <c r="J7" t="s">
+        <v>107</v>
+      </c>
       <c r="L7" s="7" t="s">
         <v>7</v>
       </c>
@@ -1920,7 +1940,9 @@
       <c r="I8" t="s">
         <v>42</v>
       </c>
-      <c r="J8"/>
+      <c r="J8" t="s">
+        <v>107</v>
+      </c>
       <c r="L8" s="7" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Cleaner up code. Added radius setup, total length monitoring, language and relays active saved to eeprom
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8824" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10188" uniqueCount="176">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -528,6 +528,21 @@
   </si>
   <si>
     <t xml:space="preserve">.",_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relays active</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Releji aktivni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radius</t>
   </si>
 </sst>
 </file>
@@ -2053,10 +2068,10 @@
         <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="G3" t="s">
-        <v>43</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4">
@@ -2073,10 +2088,10 @@
         <v>46</v>
       </c>
       <c r="F4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" t="s">
         <v>48</v>
-      </c>
-      <c r="G4" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="5">
@@ -2193,10 +2208,10 @@
         <v>46</v>
       </c>
       <c r="F10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" t="s">
         <v>59</v>
-      </c>
-      <c r="G10" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="11">
@@ -2213,10 +2228,10 @@
         <v>46</v>
       </c>
       <c r="F11" t="s">
+        <v>108</v>
+      </c>
+      <c r="G11" t="s">
         <v>72</v>
-      </c>
-      <c r="G11" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="12">
@@ -2273,10 +2288,10 @@
         <v>46</v>
       </c>
       <c r="F14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G14" t="s">
         <v>70</v>
-      </c>
-      <c r="G14" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="15">
@@ -2293,10 +2308,10 @@
         <v>46</v>
       </c>
       <c r="F15" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" t="s">
         <v>74</v>
-      </c>
-      <c r="G15" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="16">
@@ -2313,10 +2328,10 @@
         <v>46</v>
       </c>
       <c r="F16" t="s">
+        <v>80</v>
+      </c>
+      <c r="G16" t="s">
         <v>76</v>
-      </c>
-      <c r="G16" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="17">
@@ -2333,10 +2348,10 @@
         <v>46</v>
       </c>
       <c r="F17" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" t="s">
         <v>59</v>
-      </c>
-      <c r="G17" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="18">
@@ -2353,10 +2368,10 @@
         <v>46</v>
       </c>
       <c r="F18" t="s">
+        <v>108</v>
+      </c>
+      <c r="G18" t="s">
         <v>72</v>
-      </c>
-      <c r="G18" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="19">
@@ -2413,10 +2428,10 @@
         <v>46</v>
       </c>
       <c r="F21" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" t="s">
         <v>59</v>
-      </c>
-      <c r="G21" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="22">
@@ -2433,10 +2448,10 @@
         <v>46</v>
       </c>
       <c r="F22" t="s">
+        <v>108</v>
+      </c>
+      <c r="G22" t="s">
         <v>72</v>
-      </c>
-      <c r="G22" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="23">
@@ -2493,10 +2508,10 @@
         <v>46</v>
       </c>
       <c r="F25" t="s">
+        <v>60</v>
+      </c>
+      <c r="G25" t="s">
         <v>59</v>
-      </c>
-      <c r="G25" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="26">
@@ -2513,10 +2528,10 @@
         <v>46</v>
       </c>
       <c r="F26" t="s">
+        <v>108</v>
+      </c>
+      <c r="G26" t="s">
         <v>72</v>
-      </c>
-      <c r="G26" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="27">
@@ -2573,10 +2588,10 @@
         <v>46</v>
       </c>
       <c r="F29" t="s">
+        <v>158</v>
+      </c>
+      <c r="G29" t="s">
         <v>109</v>
-      </c>
-      <c r="G29" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="30">
@@ -2693,10 +2708,10 @@
         <v>46</v>
       </c>
       <c r="F35" t="s">
+        <v>80</v>
+      </c>
+      <c r="G35" t="s">
         <v>116</v>
-      </c>
-      <c r="G35" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="36">
@@ -2713,10 +2728,10 @@
         <v>46</v>
       </c>
       <c r="F36" t="s">
+        <v>85</v>
+      </c>
+      <c r="G36" t="s">
         <v>118</v>
-      </c>
-      <c r="G36" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="37">
@@ -2733,10 +2748,10 @@
         <v>46</v>
       </c>
       <c r="F37" t="s">
+        <v>122</v>
+      </c>
+      <c r="G37" t="s">
         <v>133</v>
-      </c>
-      <c r="G37" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="38">
@@ -2753,10 +2768,10 @@
         <v>46</v>
       </c>
       <c r="F38" t="s">
+        <v>125</v>
+      </c>
+      <c r="G38" t="s">
         <v>134</v>
-      </c>
-      <c r="G38" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="39">
@@ -2773,10 +2788,10 @@
         <v>46</v>
       </c>
       <c r="F39" t="s">
+        <v>128</v>
+      </c>
+      <c r="G39" t="s">
         <v>127</v>
-      </c>
-      <c r="G39" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="40">
@@ -2793,10 +2808,10 @@
         <v>46</v>
       </c>
       <c r="F40" t="s">
+        <v>137</v>
+      </c>
+      <c r="G40" t="s">
         <v>136</v>
-      </c>
-      <c r="G40" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="41">
@@ -2813,10 +2828,10 @@
         <v>46</v>
       </c>
       <c r="F41" t="s">
+        <v>140</v>
+      </c>
+      <c r="G41" t="s">
         <v>139</v>
-      </c>
-      <c r="G41" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="42">
@@ -2853,10 +2868,10 @@
         <v>46</v>
       </c>
       <c r="F43" t="s">
+        <v>107</v>
+      </c>
+      <c r="G43" t="s">
         <v>52</v>
-      </c>
-      <c r="G43" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="44">
@@ -3033,10 +3048,10 @@
         <v>46</v>
       </c>
       <c r="F52" t="s">
+        <v>159</v>
+      </c>
+      <c r="G52" t="s">
         <v>157</v>
-      </c>
-      <c r="G52" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="53">
@@ -3053,10 +3068,10 @@
         <v>46</v>
       </c>
       <c r="F53" t="s">
+        <v>162</v>
+      </c>
+      <c r="G53" t="s">
         <v>161</v>
-      </c>
-      <c r="G53" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="54">
@@ -3073,10 +3088,50 @@
         <v>46</v>
       </c>
       <c r="F54" t="s">
+        <v>165</v>
+      </c>
+      <c r="G54" t="s">
         <v>164</v>
       </c>
-      <c r="G54" t="s">
-        <v>165</v>
+    </row>
+    <row r="55">
+      <c r="B55" t="s">
+        <v>171</v>
+      </c>
+      <c r="C55" t="s">
+        <v>38</v>
+      </c>
+      <c r="D55" t="s">
+        <v>51</v>
+      </c>
+      <c r="E55" t="s">
+        <v>46</v>
+      </c>
+      <c r="F55" t="s">
+        <v>173</v>
+      </c>
+      <c r="G55" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="B56" t="s">
+        <v>174</v>
+      </c>
+      <c r="C56" t="s">
+        <v>38</v>
+      </c>
+      <c r="D56" t="s">
+        <v>51</v>
+      </c>
+      <c r="E56" t="s">
+        <v>46</v>
+      </c>
+      <c r="F56" t="s">
+        <v>175</v>
+      </c>
+      <c r="G56" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Part 2 of latest GRBL laser control commit. Contain HAL files
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10188" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16276" uniqueCount="249">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -543,6 +543,225 @@
   </si>
   <si>
     <t xml:space="preserve">Radius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId59</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;uartConsoleBfr&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId63</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;uartConsoleBfr_0&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId64</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;uartConsoleBfr_1&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId65</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;uartConsoleBfr_2&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId66</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;uartConsoleBfr_3&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId67</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;uartConsoleBfr_4&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId68</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;uartConsoleBfr_5&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alpha: °</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alpha:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beta: &lt;beta&gt; °</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">širina: &lt;beta&gt; °</t>
+  </si>
+  <si>
+    <t xml:space="preserve">width: &lt;beta&gt; °</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hitrost: &lt;beta&gt; mm/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f. rate: &lt;beta&gt; mm/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.",°</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.",_°</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alpha [°]:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">širina [mm]:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">width [mm]:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hitrost [mm/s]:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f. rate [mm/s]:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beta [°]:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Save 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Save 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Save 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alpha: [°]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alpha: &lt;alpha&gt;°</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">širina: &lt;width&gt;mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">width: &lt;width&gt;mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId92</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hitrost: &lt;feedrate&gt;mm/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f. rate: &lt;feedrate&gt;mm/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beta: &lt;beta&gt;°</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x0 [mm]:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y0 [mm]:</t>
   </si>
 </sst>
 </file>
@@ -1785,7 +2004,7 @@
         <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>166</v>
+        <v>201</v>
       </c>
       <c r="H4"/>
       <c r="I4" t="s">
@@ -1827,7 +2046,7 @@
         <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>166</v>
+        <v>201</v>
       </c>
       <c r="H5"/>
       <c r="I5" t="s">
@@ -1867,7 +2086,7 @@
         <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>170</v>
+        <v>202</v>
       </c>
       <c r="H6"/>
       <c r="I6" t="s">
@@ -1907,7 +2126,7 @@
         <v>17</v>
       </c>
       <c r="G7" t="s">
-        <v>166</v>
+        <v>201</v>
       </c>
       <c r="H7"/>
       <c r="I7" t="s">
@@ -1949,7 +2168,7 @@
         <v>17</v>
       </c>
       <c r="G8" t="s">
-        <v>166</v>
+        <v>201</v>
       </c>
       <c r="H8"/>
       <c r="I8" t="s">
@@ -3134,6 +3353,686 @@
         <v>175</v>
       </c>
     </row>
+    <row r="57">
+      <c r="B57" t="s">
+        <v>178</v>
+      </c>
+      <c r="C57" t="s">
+        <v>41</v>
+      </c>
+      <c r="D57" t="s">
+        <v>51</v>
+      </c>
+      <c r="E57" t="s">
+        <v>46</v>
+      </c>
+      <c r="F57" t="s">
+        <v>177</v>
+      </c>
+      <c r="G57" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" t="s">
+        <v>180</v>
+      </c>
+      <c r="C58" t="s">
+        <v>41</v>
+      </c>
+      <c r="D58" t="s">
+        <v>51</v>
+      </c>
+      <c r="E58" t="s">
+        <v>46</v>
+      </c>
+      <c r="F58" t="s">
+        <v>177</v>
+      </c>
+      <c r="G58" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59" t="s">
+        <v>182</v>
+      </c>
+      <c r="C59" t="s">
+        <v>41</v>
+      </c>
+      <c r="D59" t="s">
+        <v>51</v>
+      </c>
+      <c r="E59" t="s">
+        <v>46</v>
+      </c>
+      <c r="F59" t="s">
+        <v>177</v>
+      </c>
+      <c r="G59" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="B60" t="s">
+        <v>184</v>
+      </c>
+      <c r="C60" t="s">
+        <v>41</v>
+      </c>
+      <c r="D60" t="s">
+        <v>51</v>
+      </c>
+      <c r="E60" t="s">
+        <v>46</v>
+      </c>
+      <c r="F60" t="s">
+        <v>177</v>
+      </c>
+      <c r="G60" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="B61" t="s">
+        <v>186</v>
+      </c>
+      <c r="C61" t="s">
+        <v>41</v>
+      </c>
+      <c r="D61" t="s">
+        <v>51</v>
+      </c>
+      <c r="E61" t="s">
+        <v>46</v>
+      </c>
+      <c r="F61" t="s">
+        <v>177</v>
+      </c>
+      <c r="G61" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="B62" t="s">
+        <v>188</v>
+      </c>
+      <c r="C62" t="s">
+        <v>41</v>
+      </c>
+      <c r="D62" t="s">
+        <v>51</v>
+      </c>
+      <c r="E62" t="s">
+        <v>46</v>
+      </c>
+      <c r="F62" t="s">
+        <v>177</v>
+      </c>
+      <c r="G62" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="B63" t="s">
+        <v>190</v>
+      </c>
+      <c r="C63" t="s">
+        <v>40</v>
+      </c>
+      <c r="D63" t="s">
+        <v>82</v>
+      </c>
+      <c r="E63" t="s">
+        <v>46</v>
+      </c>
+      <c r="F63" t="s">
+        <v>191</v>
+      </c>
+      <c r="G63" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="B64" t="s">
+        <v>195</v>
+      </c>
+      <c r="C64" t="s">
+        <v>40</v>
+      </c>
+      <c r="D64" t="s">
+        <v>82</v>
+      </c>
+      <c r="E64" t="s">
+        <v>46</v>
+      </c>
+      <c r="F64" t="s">
+        <v>204</v>
+      </c>
+      <c r="G64" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="B65" t="s">
+        <v>198</v>
+      </c>
+      <c r="C65" t="s">
+        <v>38</v>
+      </c>
+      <c r="D65" t="s">
+        <v>82</v>
+      </c>
+      <c r="E65" t="s">
+        <v>46</v>
+      </c>
+      <c r="F65" t="s">
+        <v>206</v>
+      </c>
+      <c r="G65" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="B66" t="s">
+        <v>208</v>
+      </c>
+      <c r="C66" t="s">
+        <v>40</v>
+      </c>
+      <c r="D66" t="s">
+        <v>82</v>
+      </c>
+      <c r="E66" t="s">
+        <v>46</v>
+      </c>
+      <c r="F66" t="s">
+        <v>209</v>
+      </c>
+      <c r="G66" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="B67" t="s">
+        <v>210</v>
+      </c>
+      <c r="C67" t="s">
+        <v>40</v>
+      </c>
+      <c r="D67" t="s">
+        <v>51</v>
+      </c>
+      <c r="E67" t="s">
+        <v>46</v>
+      </c>
+      <c r="F67" t="s">
+        <v>145</v>
+      </c>
+      <c r="G67" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="B68" t="s">
+        <v>211</v>
+      </c>
+      <c r="C68" t="s">
+        <v>40</v>
+      </c>
+      <c r="D68" t="s">
+        <v>51</v>
+      </c>
+      <c r="E68" t="s">
+        <v>46</v>
+      </c>
+      <c r="F68" t="s">
+        <v>145</v>
+      </c>
+      <c r="G68" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="B69" t="s">
+        <v>212</v>
+      </c>
+      <c r="C69" t="s">
+        <v>40</v>
+      </c>
+      <c r="D69" t="s">
+        <v>51</v>
+      </c>
+      <c r="E69" t="s">
+        <v>46</v>
+      </c>
+      <c r="F69" t="s">
+        <v>145</v>
+      </c>
+      <c r="G69" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="B70" t="s">
+        <v>213</v>
+      </c>
+      <c r="C70" t="s">
+        <v>40</v>
+      </c>
+      <c r="D70" t="s">
+        <v>51</v>
+      </c>
+      <c r="E70" t="s">
+        <v>46</v>
+      </c>
+      <c r="F70" t="s">
+        <v>145</v>
+      </c>
+      <c r="G70" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="B71" t="s">
+        <v>214</v>
+      </c>
+      <c r="C71" t="s">
+        <v>40</v>
+      </c>
+      <c r="D71" t="s">
+        <v>51</v>
+      </c>
+      <c r="E71" t="s">
+        <v>46</v>
+      </c>
+      <c r="F71" t="s">
+        <v>145</v>
+      </c>
+      <c r="G71" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="B72" t="s">
+        <v>215</v>
+      </c>
+      <c r="C72" t="s">
+        <v>40</v>
+      </c>
+      <c r="D72" t="s">
+        <v>51</v>
+      </c>
+      <c r="E72" t="s">
+        <v>46</v>
+      </c>
+      <c r="F72" t="s">
+        <v>145</v>
+      </c>
+      <c r="G72" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="B73" t="s">
+        <v>216</v>
+      </c>
+      <c r="C73" t="s">
+        <v>38</v>
+      </c>
+      <c r="D73" t="s">
+        <v>82</v>
+      </c>
+      <c r="E73" t="s">
+        <v>46</v>
+      </c>
+      <c r="F73" t="s">
+        <v>232</v>
+      </c>
+      <c r="G73" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="B74" t="s">
+        <v>217</v>
+      </c>
+      <c r="C74" t="s">
+        <v>38</v>
+      </c>
+      <c r="D74" t="s">
+        <v>82</v>
+      </c>
+      <c r="E74" t="s">
+        <v>46</v>
+      </c>
+      <c r="F74" t="s">
+        <v>204</v>
+      </c>
+      <c r="G74" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="B75" t="s">
+        <v>218</v>
+      </c>
+      <c r="C75" t="s">
+        <v>38</v>
+      </c>
+      <c r="D75" t="s">
+        <v>82</v>
+      </c>
+      <c r="E75" t="s">
+        <v>46</v>
+      </c>
+      <c r="F75" t="s">
+        <v>206</v>
+      </c>
+      <c r="G75" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="B76" t="s">
+        <v>219</v>
+      </c>
+      <c r="C76" t="s">
+        <v>38</v>
+      </c>
+      <c r="D76" t="s">
+        <v>82</v>
+      </c>
+      <c r="E76" t="s">
+        <v>46</v>
+      </c>
+      <c r="F76" t="s">
+        <v>209</v>
+      </c>
+      <c r="G76" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="B77" t="s">
+        <v>220</v>
+      </c>
+      <c r="C77" t="s">
+        <v>38</v>
+      </c>
+      <c r="D77" t="s">
+        <v>45</v>
+      </c>
+      <c r="E77" t="s">
+        <v>46</v>
+      </c>
+      <c r="F77" t="s">
+        <v>221</v>
+      </c>
+      <c r="G77" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="B78" t="s">
+        <v>222</v>
+      </c>
+      <c r="C78" t="s">
+        <v>38</v>
+      </c>
+      <c r="D78" t="s">
+        <v>45</v>
+      </c>
+      <c r="E78" t="s">
+        <v>46</v>
+      </c>
+      <c r="F78" t="s">
+        <v>223</v>
+      </c>
+      <c r="G78" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="B79" t="s">
+        <v>224</v>
+      </c>
+      <c r="C79" t="s">
+        <v>38</v>
+      </c>
+      <c r="D79" t="s">
+        <v>45</v>
+      </c>
+      <c r="E79" t="s">
+        <v>46</v>
+      </c>
+      <c r="F79" t="s">
+        <v>225</v>
+      </c>
+      <c r="G79" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="B80" t="s">
+        <v>226</v>
+      </c>
+      <c r="C80" t="s">
+        <v>38</v>
+      </c>
+      <c r="D80" t="s">
+        <v>45</v>
+      </c>
+      <c r="E80" t="s">
+        <v>46</v>
+      </c>
+      <c r="F80" t="s">
+        <v>227</v>
+      </c>
+      <c r="G80" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="B81" t="s">
+        <v>228</v>
+      </c>
+      <c r="C81" t="s">
+        <v>38</v>
+      </c>
+      <c r="D81" t="s">
+        <v>45</v>
+      </c>
+      <c r="E81" t="s">
+        <v>46</v>
+      </c>
+      <c r="F81" t="s">
+        <v>229</v>
+      </c>
+      <c r="G81" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="B82" t="s">
+        <v>230</v>
+      </c>
+      <c r="C82" t="s">
+        <v>38</v>
+      </c>
+      <c r="D82" t="s">
+        <v>45</v>
+      </c>
+      <c r="E82" t="s">
+        <v>46</v>
+      </c>
+      <c r="F82" t="s">
+        <v>231</v>
+      </c>
+      <c r="G82" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="B83" t="s">
+        <v>233</v>
+      </c>
+      <c r="C83" t="s">
+        <v>40</v>
+      </c>
+      <c r="D83" t="s">
+        <v>51</v>
+      </c>
+      <c r="E83" t="s">
+        <v>46</v>
+      </c>
+      <c r="F83" t="s">
+        <v>234</v>
+      </c>
+      <c r="G83" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="B84" t="s">
+        <v>235</v>
+      </c>
+      <c r="C84" t="s">
+        <v>40</v>
+      </c>
+      <c r="D84" t="s">
+        <v>51</v>
+      </c>
+      <c r="E84" t="s">
+        <v>46</v>
+      </c>
+      <c r="F84" t="s">
+        <v>236</v>
+      </c>
+      <c r="G84" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="B85" t="s">
+        <v>238</v>
+      </c>
+      <c r="C85" t="s">
+        <v>40</v>
+      </c>
+      <c r="D85" t="s">
+        <v>51</v>
+      </c>
+      <c r="E85" t="s">
+        <v>46</v>
+      </c>
+      <c r="F85" t="s">
+        <v>239</v>
+      </c>
+      <c r="G85" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="B86" t="s">
+        <v>241</v>
+      </c>
+      <c r="C86" t="s">
+        <v>40</v>
+      </c>
+      <c r="D86" t="s">
+        <v>51</v>
+      </c>
+      <c r="E86" t="s">
+        <v>46</v>
+      </c>
+      <c r="F86" t="s">
+        <v>242</v>
+      </c>
+      <c r="G86" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="B87" t="s">
+        <v>243</v>
+      </c>
+      <c r="C87" t="s">
+        <v>40</v>
+      </c>
+      <c r="D87" t="s">
+        <v>51</v>
+      </c>
+      <c r="E87" t="s">
+        <v>46</v>
+      </c>
+      <c r="F87" t="s">
+        <v>145</v>
+      </c>
+      <c r="G87" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="B88" t="s">
+        <v>244</v>
+      </c>
+      <c r="C88" t="s">
+        <v>40</v>
+      </c>
+      <c r="D88" t="s">
+        <v>51</v>
+      </c>
+      <c r="E88" t="s">
+        <v>46</v>
+      </c>
+      <c r="F88" t="s">
+        <v>145</v>
+      </c>
+      <c r="G88" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="B89" t="s">
+        <v>245</v>
+      </c>
+      <c r="C89" t="s">
+        <v>40</v>
+      </c>
+      <c r="D89" t="s">
+        <v>82</v>
+      </c>
+      <c r="E89" t="s">
+        <v>46</v>
+      </c>
+      <c r="F89" t="s">
+        <v>246</v>
+      </c>
+      <c r="G89" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="B90" t="s">
+        <v>247</v>
+      </c>
+      <c r="C90" t="s">
+        <v>40</v>
+      </c>
+      <c r="D90" t="s">
+        <v>82</v>
+      </c>
+      <c r="E90" t="s">
+        <v>46</v>
+      </c>
+      <c r="F90" t="s">
+        <v>248</v>
+      </c>
+      <c r="G90" t="s">
+        <v>248</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
A lot of changes. Not done yet.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16276" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22308" uniqueCount="264">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -762,6 +762,51 @@
   </si>
   <si>
     <t xml:space="preserve">y0 [mm]:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATUSMSG_SETTINGS_UART_TX_ERR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Napaka pri UART TX komunikaciji.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UART TX communication error.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATUSMSG_SETTINGS_UART_TX_NOT_OKED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRBL je zavrnil G-komando.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRBL denied G-code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[rez / na 0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[cut / to 0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0020-0x007F,0x00C0-0x00FF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0020-0x007F,0x00C0-0x00FF,0x0018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId105</t>
   </si>
 </sst>
 </file>
@@ -2077,7 +2122,7 @@
         <v>77</v>
       </c>
       <c r="D6">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -2090,7 +2135,7 @@
       </c>
       <c r="H6"/>
       <c r="I6" t="s">
-        <v>167</v>
+        <v>259</v>
       </c>
       <c r="J6" t="s">
         <v>107</v>
@@ -3687,7 +3732,7 @@
         <v>46</v>
       </c>
       <c r="F73" t="s">
-        <v>232</v>
+        <v>203</v>
       </c>
       <c r="G73" t="s">
         <v>203</v>
@@ -4031,6 +4076,146 @@
       </c>
       <c r="G90" t="s">
         <v>248</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="B91" t="s">
+        <v>249</v>
+      </c>
+      <c r="C91" t="s">
+        <v>38</v>
+      </c>
+      <c r="D91" t="s">
+        <v>51</v>
+      </c>
+      <c r="E91" t="s">
+        <v>46</v>
+      </c>
+      <c r="F91" t="s">
+        <v>250</v>
+      </c>
+      <c r="G91" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="B92" t="s">
+        <v>252</v>
+      </c>
+      <c r="C92" t="s">
+        <v>38</v>
+      </c>
+      <c r="D92" t="s">
+        <v>51</v>
+      </c>
+      <c r="E92" t="s">
+        <v>46</v>
+      </c>
+      <c r="F92" t="s">
+        <v>253</v>
+      </c>
+      <c r="G92" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="B93" t="s">
+        <v>255</v>
+      </c>
+      <c r="C93" t="s">
+        <v>38</v>
+      </c>
+      <c r="D93" t="s">
+        <v>51</v>
+      </c>
+      <c r="E93" t="s">
+        <v>46</v>
+      </c>
+      <c r="F93" t="s">
+        <v>256</v>
+      </c>
+      <c r="G93" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="B94" t="s">
+        <v>260</v>
+      </c>
+      <c r="C94" t="s">
+        <v>41</v>
+      </c>
+      <c r="D94" t="s">
+        <v>51</v>
+      </c>
+      <c r="E94" t="s">
+        <v>46</v>
+      </c>
+      <c r="F94" t="s">
+        <v>177</v>
+      </c>
+      <c r="G94" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="B95" t="s">
+        <v>261</v>
+      </c>
+      <c r="C95" t="s">
+        <v>41</v>
+      </c>
+      <c r="D95" t="s">
+        <v>51</v>
+      </c>
+      <c r="E95" t="s">
+        <v>46</v>
+      </c>
+      <c r="F95" t="s">
+        <v>177</v>
+      </c>
+      <c r="G95" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="B96" t="s">
+        <v>262</v>
+      </c>
+      <c r="C96" t="s">
+        <v>41</v>
+      </c>
+      <c r="D96" t="s">
+        <v>51</v>
+      </c>
+      <c r="E96" t="s">
+        <v>46</v>
+      </c>
+      <c r="F96" t="s">
+        <v>177</v>
+      </c>
+      <c r="G96" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="B97" t="s">
+        <v>263</v>
+      </c>
+      <c r="C97" t="s">
+        <v>41</v>
+      </c>
+      <c r="D97" t="s">
+        <v>51</v>
+      </c>
+      <c r="E97" t="s">
+        <v>46</v>
+      </c>
+      <c r="F97" t="s">
+        <v>177</v>
+      </c>
+      <c r="G97" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest modification that includes GRBL control
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22308" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38352" uniqueCount="373">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -807,6 +807,415 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0020-0x007F,0x00C0-0x00FF,0x0018,0x000D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obseg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Circumference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId108</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enkoder
+p.n.o.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encoder
+p.p.r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upora.
+radij</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use 
+radius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enkoder
+p.n.o.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encoder
+p.p.r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upora.
+radij</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use 
+radius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hitrost [mm/min]:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f. rate [mm/min]:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hitrost: &lt;feedrate&gt;mm/min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f. rate: &lt;feedrate&gt;mm/min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enkoder
+p.n.o.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encoder
+p.p.r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uporabi
+radij</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use 
+radius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enkoder
+p.n.o.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encoder
+p.p.r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uporabi
+radij</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use 
+radius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATUSMSG_ORIGIN_UPDATED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Izhodisce in domaca pozicija posodobljeni.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Origin and home position updated.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enkoder
+p.n.o.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encoder
+p.p.r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uporabi
+radij</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use 
+radius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enkoder
+p.n.o.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encoder
+p.p.r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uporabi
+radij</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use 
+radius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   rez [mm/min]:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enkoder
+p.n.o.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encoder
+p.p.r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uporabi
+radij</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use 
+radius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proiz.: &lt;feedrate&gt;mm/min</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> prod.: &lt;velocity&gt;mm/min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enkoder
+p.n.o.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encoder
+p.p.r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uporabi
+radij</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use 
+radius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enkoder
+p.n.o.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encoder
+p.p.r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uporabi
+radij</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use 
+radius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRBL kontroler povezan. 
+Nadaljujem z iskanjem (0,0)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRBL controller connected. 
+Proceed with homing?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enkoder
+p.n.o.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encoder
+p.p.r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uporabi
+radij</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use 
+radius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRBL kontroler povezan. 
+Nadaljujem z iskanjem (0,0)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRBL controller connected. 
+Proceed with homing?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enkoder
+p.n.o.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encoder
+p.p.r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uporabi
+radij</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use 
+radius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRBL kontroler povezan. 
+Nadaljujem z iskanjem (0,0)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRBL controller connected. 
+Proceed with homing?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enkoder
+p.n.o.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encoder
+p.p.r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uporabi
+radij</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use 
+radius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRBL kontroler povezan. 
+Nadaljujem z iskanjem (0,0)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRBL controller connected. 
+Proceed with homing?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enkoder
+p.n.o.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encoder
+p.p.r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uporabi
+radij</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use 
+radius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRBL kontroler povezan. 
+Nadaljujem z iskanjem (0,0)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRBL controller connected. 
+Proceed with homing?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enkoder
+p.n.o.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encoder
+p.p.r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uporabi
+radij</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use 
+radius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRBL kontroler povezan. 
+Nadaljujem z iskanjem (0,0)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRBL controller connected. 
+Proceed with homing?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.",°βα</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shrani 
+1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Save 
+1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shrani
+2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Save 
+2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nalozi
+1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load 
+1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nalozi
+2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load 
+2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shrani
+3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Save 
+3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nalozi
+3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load 
+3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">α rez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">α cut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laser
+Console</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laser Console</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laser 
+Konzola</t>
   </si>
 </sst>
 </file>
@@ -2049,11 +2458,11 @@
         <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>201</v>
+        <v>353</v>
       </c>
       <c r="H4"/>
       <c r="I4" t="s">
-        <v>42</v>
+        <v>352</v>
       </c>
       <c r="J4" t="s">
         <v>107</v>
@@ -2135,7 +2544,7 @@
       </c>
       <c r="H6"/>
       <c r="I6" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="J6" t="s">
         <v>107</v>
@@ -3772,10 +4181,10 @@
         <v>46</v>
       </c>
       <c r="F75" t="s">
-        <v>206</v>
+        <v>303</v>
       </c>
       <c r="G75" t="s">
-        <v>207</v>
+        <v>281</v>
       </c>
     </row>
     <row r="76">
@@ -3812,10 +4221,10 @@
         <v>46</v>
       </c>
       <c r="F77" t="s">
-        <v>221</v>
+        <v>354</v>
       </c>
       <c r="G77" t="s">
-        <v>221</v>
+        <v>355</v>
       </c>
     </row>
     <row r="78">
@@ -3832,10 +4241,10 @@
         <v>46</v>
       </c>
       <c r="F78" t="s">
-        <v>223</v>
+        <v>356</v>
       </c>
       <c r="G78" t="s">
-        <v>223</v>
+        <v>357</v>
       </c>
     </row>
     <row r="79">
@@ -3852,10 +4261,10 @@
         <v>46</v>
       </c>
       <c r="F79" t="s">
-        <v>225</v>
+        <v>358</v>
       </c>
       <c r="G79" t="s">
-        <v>225</v>
+        <v>359</v>
       </c>
     </row>
     <row r="80">
@@ -3872,10 +4281,10 @@
         <v>46</v>
       </c>
       <c r="F80" t="s">
-        <v>227</v>
+        <v>360</v>
       </c>
       <c r="G80" t="s">
-        <v>227</v>
+        <v>361</v>
       </c>
     </row>
     <row r="81">
@@ -3892,10 +4301,10 @@
         <v>46</v>
       </c>
       <c r="F81" t="s">
-        <v>229</v>
+        <v>362</v>
       </c>
       <c r="G81" t="s">
-        <v>229</v>
+        <v>363</v>
       </c>
     </row>
     <row r="82">
@@ -3912,10 +4321,10 @@
         <v>46</v>
       </c>
       <c r="F82" t="s">
-        <v>231</v>
+        <v>364</v>
       </c>
       <c r="G82" t="s">
-        <v>231</v>
+        <v>365</v>
       </c>
     </row>
     <row r="83">
@@ -3972,10 +4381,10 @@
         <v>46</v>
       </c>
       <c r="F85" t="s">
-        <v>239</v>
+        <v>282</v>
       </c>
       <c r="G85" t="s">
-        <v>240</v>
+        <v>283</v>
       </c>
     </row>
     <row r="86">
@@ -4216,6 +4625,206 @@
       </c>
       <c r="G97" t="s">
         <v>189</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="B98" t="s">
+        <v>265</v>
+      </c>
+      <c r="C98" t="s">
+        <v>40</v>
+      </c>
+      <c r="D98" t="s">
+        <v>51</v>
+      </c>
+      <c r="E98" t="s">
+        <v>46</v>
+      </c>
+      <c r="F98" t="s">
+        <v>118</v>
+      </c>
+      <c r="G98" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="B99" t="s">
+        <v>266</v>
+      </c>
+      <c r="C99" t="s">
+        <v>38</v>
+      </c>
+      <c r="D99" t="s">
+        <v>82</v>
+      </c>
+      <c r="E99" t="s">
+        <v>46</v>
+      </c>
+      <c r="F99" t="s">
+        <v>267</v>
+      </c>
+      <c r="G99" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="B100" t="s">
+        <v>269</v>
+      </c>
+      <c r="C100" t="s">
+        <v>40</v>
+      </c>
+      <c r="D100" t="s">
+        <v>51</v>
+      </c>
+      <c r="E100" t="s">
+        <v>46</v>
+      </c>
+      <c r="F100" t="s">
+        <v>145</v>
+      </c>
+      <c r="G100" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="B101" t="s">
+        <v>270</v>
+      </c>
+      <c r="C101" t="s">
+        <v>38</v>
+      </c>
+      <c r="D101" t="s">
+        <v>82</v>
+      </c>
+      <c r="E101" t="s">
+        <v>46</v>
+      </c>
+      <c r="F101" t="s">
+        <v>271</v>
+      </c>
+      <c r="G101" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="B102" t="s">
+        <v>273</v>
+      </c>
+      <c r="C102" t="s">
+        <v>38</v>
+      </c>
+      <c r="D102" t="s">
+        <v>45</v>
+      </c>
+      <c r="E102" t="s">
+        <v>46</v>
+      </c>
+      <c r="F102" t="s">
+        <v>286</v>
+      </c>
+      <c r="G102" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="B103" t="s">
+        <v>292</v>
+      </c>
+      <c r="C103" t="s">
+        <v>38</v>
+      </c>
+      <c r="D103" t="s">
+        <v>51</v>
+      </c>
+      <c r="E103" t="s">
+        <v>46</v>
+      </c>
+      <c r="F103" t="s">
+        <v>293</v>
+      </c>
+      <c r="G103" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="B104" t="s">
+        <v>308</v>
+      </c>
+      <c r="C104" t="s">
+        <v>40</v>
+      </c>
+      <c r="D104" t="s">
+        <v>51</v>
+      </c>
+      <c r="E104" t="s">
+        <v>46</v>
+      </c>
+      <c r="F104" t="s">
+        <v>309</v>
+      </c>
+      <c r="G104" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="B105" t="s">
+        <v>319</v>
+      </c>
+      <c r="C105" t="s">
+        <v>38</v>
+      </c>
+      <c r="D105" t="s">
+        <v>45</v>
+      </c>
+      <c r="E105" t="s">
+        <v>46</v>
+      </c>
+      <c r="F105" t="s">
+        <v>320</v>
+      </c>
+      <c r="G105" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="B106" t="s">
+        <v>366</v>
+      </c>
+      <c r="C106" t="s">
+        <v>38</v>
+      </c>
+      <c r="D106" t="s">
+        <v>45</v>
+      </c>
+      <c r="E106" t="s">
+        <v>46</v>
+      </c>
+      <c r="F106" t="s">
+        <v>367</v>
+      </c>
+      <c r="G106" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="B107" t="s">
+        <v>369</v>
+      </c>
+      <c r="C107" t="s">
+        <v>38</v>
+      </c>
+      <c r="D107" t="s">
+        <v>45</v>
+      </c>
+      <c r="E107" t="s">
+        <v>46</v>
+      </c>
+      <c r="F107" t="s">
+        <v>372</v>
+      </c>
+      <c r="G107" t="s">
+        <v>370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>